<commit_message>
Updated requirements.txt and other bits in repo
</commit_message>
<xml_diff>
--- a/misc/Cansat Components.xlsx
+++ b/misc/Cansat Components.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Python\cansat-24\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30CEFF1D-5653-46E0-80BA-8F50FC948310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74DFC04A-4856-4700-826D-3757B27FC284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D8B62C31-7F45-4FA9-B0B4-7D8DA4C4CD4B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{D8B62C31-7F45-4FA9-B0B4-7D8DA4C4CD4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Dimensions" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="47">
   <si>
     <t>Component</t>
   </si>
@@ -176,6 +176,9 @@
   </si>
   <si>
     <t>Discount (-)</t>
+  </si>
+  <si>
+    <t>USB-C Extension/Mount</t>
   </si>
 </sst>
 </file>
@@ -185,7 +188,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,6 +242,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -365,24 +376,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -398,9 +407,12 @@
     <xf numFmtId="44" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -735,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{355C6535-266D-4D0C-92F9-5F6725771D18}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -749,22 +761,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="9" t="s">
         <v>22</v>
       </c>
     </row>
@@ -784,137 +796,131 @@
       <c r="E2" s="3">
         <v>7</v>
       </c>
-      <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>26</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>17.8</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>4.5999999999999996</v>
       </c>
-      <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>25.5</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>25.4</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>8.1999999999999993</v>
       </c>
-      <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>19</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>19</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>8</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="7"/>
+      <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>29</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>25</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>4</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="6">
         <v>60</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="6">
         <v>36</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="6">
         <v>7</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="7"/>
+      <c r="G7" s="5"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="9"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="8">
         <v>115</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="8">
         <v>66</v>
       </c>
-      <c r="E10" s="4"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
+      <c r="A12" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -939,13 +945,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="13" t="s">
         <v>32</v>
       </c>
     </row>
@@ -961,57 +967,57 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="6" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1024,16 +1030,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2228B123-4275-49BB-84D6-D3E44895DC7A}">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="122" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="18.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="9.140625" style="1" customWidth="1"/>
     <col min="7" max="7" width="38.42578125" style="1" customWidth="1"/>
@@ -1046,194 +1052,199 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="13" t="s">
         <v>32</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="20">
+      <c r="F1" s="17">
         <f>SUM(B2:B21)</f>
-        <v>100.6</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="17">
+      <c r="B2" s="14">
         <v>11.9</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="F2" s="21">
+      <c r="F2" s="18">
         <f>SUM(B6,B5)</f>
         <v>38.4</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="18">
+      <c r="B3" s="15">
         <v>12.9</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="E3" s="19" t="s">
+      <c r="C3" s="4"/>
+      <c r="E3" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="F3" s="23">
+      <c r="F3" s="20">
         <f>F1-F2</f>
-        <v>62.199999999999996</v>
+        <v>73.599999999999994</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="18">
+      <c r="B4" s="15">
         <v>29.4</v>
       </c>
-      <c r="C4" s="5"/>
+      <c r="C4" s="4"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="18">
+      <c r="B5" s="15">
         <v>18.899999999999999</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="18">
+      <c r="B6" s="15">
         <v>19.5</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="18">
+      <c r="B7" s="15">
         <v>8</v>
       </c>
-      <c r="C7" s="13"/>
+      <c r="C7" s="10"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="15">
+        <v>11.4</v>
+      </c>
+      <c r="C8" s="10"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="13"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+      <c r="B9" s="15"/>
+      <c r="C9" s="10"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="13"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="B10" s="15"/>
+      <c r="C10" s="10"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="13"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="B11" s="15"/>
+      <c r="C11" s="10"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="13"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="B12" s="15"/>
+      <c r="C12" s="10"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="13"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="B13" s="15"/>
+      <c r="C13" s="10"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="13"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="B14" s="15"/>
+      <c r="C14" s="10"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="5"/>
-      <c r="C14" s="13"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
+      <c r="B15" s="15"/>
+      <c r="C15" s="10"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="13"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
+      <c r="B16" s="15"/>
+      <c r="C16" s="10"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="13"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
+      <c r="B17" s="15"/>
+      <c r="C17" s="10"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="13"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+      <c r="B18" s="15"/>
+      <c r="C18" s="10"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="13"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
+      <c r="B19" s="15"/>
+      <c r="C19" s="10"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="13"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
+      <c r="B20" s="15"/>
+      <c r="C20" s="10"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="13"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21" s="8"/>
-      <c r="C21" s="14"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="11"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A8" r:id="rId1" xr:uid="{1EBD4FC7-E37F-433A-88EB-0AE5641E06FC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>